<commit_message>
#78 addin upload support and lock support
</commit_message>
<xml_diff>
--- a/src/main/data/IPL-Players.xlsx
+++ b/src/main/data/IPL-Players.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/repo/Sport-fantasy-league/src/main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9848A0-7134-C04C-B8CA-F62662287C3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9BD78B-F095-2F4F-A2DD-E913207ABEFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D6C1F2CB-1571-5643-8A56-0F046E991C21}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16300" xr2:uid="{D6C1F2CB-1571-5643-8A56-0F046E991C21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="64">
   <si>
     <t>MS Dhoni</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>SRILANKA</t>
+  </si>
+  <si>
+    <t>Chennai Super Kings</t>
+  </si>
+  <si>
+    <t>Mumbai Indians</t>
   </si>
 </sst>
 </file>
@@ -617,19 +623,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A72C190F-5A67-5247-A77B-9919E3ECAC7C}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,8 +649,11 @@
       <c r="D1">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -656,8 +666,11 @@
       <c r="D2">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -670,8 +683,11 @@
       <c r="D3">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -684,8 +700,11 @@
       <c r="D4">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -698,8 +717,11 @@
       <c r="D5">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -712,8 +734,11 @@
       <c r="D6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -726,8 +751,11 @@
       <c r="D7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -740,8 +768,11 @@
       <c r="D8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -754,8 +785,11 @@
       <c r="D9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -768,8 +802,11 @@
       <c r="D10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -782,8 +819,11 @@
       <c r="D11">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -796,8 +836,11 @@
       <c r="D12">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -810,8 +853,11 @@
       <c r="D13">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -824,8 +870,11 @@
       <c r="D14">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -838,8 +887,11 @@
       <c r="D15">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -852,8 +904,11 @@
       <c r="D16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -866,8 +921,11 @@
       <c r="D17">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -880,8 +938,11 @@
       <c r="D18">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -894,8 +955,11 @@
       <c r="D19">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -908,8 +972,11 @@
       <c r="D20">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -922,8 +989,11 @@
       <c r="D21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -936,8 +1006,11 @@
       <c r="D22">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -950,8 +1023,11 @@
       <c r="D23">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -964,8 +1040,11 @@
       <c r="D24">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -978,8 +1057,11 @@
       <c r="D25">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -992,8 +1074,11 @@
       <c r="D26">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1006,8 +1091,11 @@
       <c r="D27">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -1020,8 +1108,11 @@
       <c r="D28">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>28</v>
       </c>
@@ -1034,8 +1125,11 @@
       <c r="D29">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>29</v>
       </c>
@@ -1048,8 +1142,11 @@
       <c r="D30">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>30</v>
       </c>
@@ -1062,8 +1159,11 @@
       <c r="D31">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>31</v>
       </c>
@@ -1076,8 +1176,11 @@
       <c r="D32">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>32</v>
       </c>
@@ -1090,8 +1193,11 @@
       <c r="D33">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>33</v>
       </c>
@@ -1104,8 +1210,11 @@
       <c r="D34">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>34</v>
       </c>
@@ -1118,8 +1227,11 @@
       <c r="D35">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>35</v>
       </c>
@@ -1132,8 +1244,11 @@
       <c r="D36">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>36</v>
       </c>
@@ -1146,8 +1261,11 @@
       <c r="D37">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>37</v>
       </c>
@@ -1160,8 +1278,11 @@
       <c r="D38">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>38</v>
       </c>
@@ -1174,8 +1295,11 @@
       <c r="D39">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>39</v>
       </c>
@@ -1188,8 +1312,11 @@
       <c r="D40">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>40</v>
       </c>
@@ -1202,8 +1329,11 @@
       <c r="D41">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>41</v>
       </c>
@@ -1216,8 +1346,11 @@
       <c r="D42">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>42</v>
       </c>
@@ -1230,8 +1363,11 @@
       <c r="D43">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>43</v>
       </c>
@@ -1244,8 +1380,11 @@
       <c r="D44">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>44</v>
       </c>
@@ -1258,8 +1397,11 @@
       <c r="D45">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>45</v>
       </c>
@@ -1272,8 +1414,11 @@
       <c r="D46">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>46</v>
       </c>
@@ -1286,8 +1431,11 @@
       <c r="D47">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>47</v>
       </c>
@@ -1300,8 +1448,11 @@
       <c r="D48">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>48</v>
       </c>
@@ -1314,8 +1465,11 @@
       <c r="D49">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>49</v>
       </c>
@@ -1327,6 +1481,9 @@
       </c>
       <c r="D50">
         <v>9</v>
+      </c>
+      <c r="E50" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#78 adding changes for upload player list of delhi daredevils
</commit_message>
<xml_diff>
--- a/src/main/data/IPL-Players.xlsx
+++ b/src/main/data/IPL-Players.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/repo/Sport-fantasy-league/src/main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9BD78B-F095-2F4F-A2DD-E913207ABEFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDDAB13-993C-7A46-8491-EFFB87719496}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16300" xr2:uid="{D6C1F2CB-1571-5643-8A56-0F046E991C21}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16300" activeTab="1" xr2:uid="{D6C1F2CB-1571-5643-8A56-0F046E991C21}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Delhi DareDevils" sheetId="1" r:id="rId1"/>
+    <sheet name="MI CSK" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Delhi DareDevils'!$A$1:$C$22</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="88">
   <si>
     <t>MS Dhoni</t>
   </si>
@@ -217,13 +221,85 @@
   </si>
   <si>
     <t>Mumbai Indians</t>
+  </si>
+  <si>
+    <t>Shimron Heymyer</t>
+  </si>
+  <si>
+    <t>Jason Roy</t>
+  </si>
+  <si>
+    <t>Alex Carey</t>
+  </si>
+  <si>
+    <t>Marcus Stoinis</t>
+  </si>
+  <si>
+    <t>Lalit Yadav</t>
+  </si>
+  <si>
+    <t>Chris Woakes</t>
+  </si>
+  <si>
+    <t>Mohit Sharma</t>
+  </si>
+  <si>
+    <t>Tushar Deshpande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shreyas Iyer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajinkya Rahane </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keemo Paul </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prithvi Shaw </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shikhar Dhawan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rishabh Pant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avesh Khan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ravichandran Ashwin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandeep Lamichhane </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Axax Patel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harshal Patel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ishant Sharma </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kagiso Rabada </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amit Mishra </t>
+  </si>
+  <si>
+    <t>Delhi Daredevils</t>
+  </si>
+  <si>
+    <t>NEPAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -242,6 +318,18 @@
       <sz val="11"/>
       <color rgb="FF262525"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -292,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -309,6 +397,8 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,18 +713,409 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A72C190F-5A67-5247-A77B-9919E3ECAC7C}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="1" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="5">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="5">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="5">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="5">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="5">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="5">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="5">
+        <v>8.5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="5">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="5">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="5">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="6">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="5">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="5">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="5">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="5">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="5">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="5">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="5">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="5">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="5">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C22" xr:uid="{E5A364D2-3CE8-8642-9413-35E21F4CF151}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EAE61C-B86B-1A43-86DD-0D679D0182AB}">
+  <dimension ref="A1:E50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
#79 adding last score and playr list
</commit_message>
<xml_diff>
--- a/src/main/data/IPL-Players.xlsx
+++ b/src/main/data/IPL-Players.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/repo/Sport-fantasy-league/src/main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDDAB13-993C-7A46-8491-EFFB87719496}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D8CD3F-9F6A-6C4A-B09B-B0D475FCCA32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16300" activeTab="1" xr2:uid="{D6C1F2CB-1571-5643-8A56-0F046E991C21}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16300" activeTab="6" xr2:uid="{D6C1F2CB-1571-5643-8A56-0F046E991C21}"/>
   </bookViews>
   <sheets>
     <sheet name="Delhi DareDevils" sheetId="1" r:id="rId1"/>
-    <sheet name="MI CSK" sheetId="2" r:id="rId2"/>
+    <sheet name="RCB" sheetId="3" r:id="rId2"/>
+    <sheet name="RR" sheetId="6" r:id="rId3"/>
+    <sheet name="SRH" sheetId="7" r:id="rId4"/>
+    <sheet name="KKR" sheetId="5" r:id="rId5"/>
+    <sheet name="KXIP" sheetId="4" r:id="rId6"/>
+    <sheet name="MI CSK" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Delhi DareDevils'!$A$1:$C$22</definedName>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="210">
   <si>
     <t>MS Dhoni</t>
   </si>
@@ -289,10 +294,376 @@
     <t xml:space="preserve">Amit Mishra </t>
   </si>
   <si>
-    <t>Delhi Daredevils</t>
-  </si>
-  <si>
     <t>NEPAL</t>
+  </si>
+  <si>
+    <t>Aaron Finch</t>
+  </si>
+  <si>
+    <t>Shahbaz Ahamad</t>
+  </si>
+  <si>
+    <t>Joshua Philippe</t>
+  </si>
+  <si>
+    <t>Isuru Udana</t>
+  </si>
+  <si>
+    <t>Pavan Deshpande</t>
+  </si>
+  <si>
+    <t>Christopher Morris</t>
+  </si>
+  <si>
+    <t>Kane Richardson</t>
+  </si>
+  <si>
+    <t>Dale Steyn</t>
+  </si>
+  <si>
+    <t>Virat Kohli</t>
+  </si>
+  <si>
+    <t>AB de Villiers</t>
+  </si>
+  <si>
+    <t>Devdutt Padikkal</t>
+  </si>
+  <si>
+    <t>Gurkeerat Singh</t>
+  </si>
+  <si>
+    <t>Pathiv Patel</t>
+  </si>
+  <si>
+    <t>Pawan Negi</t>
+  </si>
+  <si>
+    <t>Shivam Dube</t>
+  </si>
+  <si>
+    <t>Moeen Ali</t>
+  </si>
+  <si>
+    <t>Mohammaed Siraj</t>
+  </si>
+  <si>
+    <t>Navdeep Saini</t>
+  </si>
+  <si>
+    <t>Umesh Yadav</t>
+  </si>
+  <si>
+    <t>Washington Sundar</t>
+  </si>
+  <si>
+    <t>Yuzvendra Chahal</t>
+  </si>
+  <si>
+    <t>Royal Challengers Bengaluru</t>
+  </si>
+  <si>
+    <t>Prabhsimran Singh</t>
+  </si>
+  <si>
+    <t>Glenn Maxwell</t>
+  </si>
+  <si>
+    <t>Chris Jordan</t>
+  </si>
+  <si>
+    <t>Deepak Hooda</t>
+  </si>
+  <si>
+    <t>James Neesham</t>
+  </si>
+  <si>
+    <t>Tajinder Dhillon</t>
+  </si>
+  <si>
+    <t>Ishan Porel</t>
+  </si>
+  <si>
+    <t>Ravi Bishnoi</t>
+  </si>
+  <si>
+    <t>Sheldon Cottrell</t>
+  </si>
+  <si>
+    <t>Kings XI Punjab</t>
+  </si>
+  <si>
+    <t>Karun Nair</t>
+  </si>
+  <si>
+    <t>Arshdeep Singh</t>
+  </si>
+  <si>
+    <t>Chris Gayle</t>
+  </si>
+  <si>
+    <t>Darshan Nalkande</t>
+  </si>
+  <si>
+    <t>Gowtham Krishnappa</t>
+  </si>
+  <si>
+    <t>Hardus Viljoen</t>
+  </si>
+  <si>
+    <t>Harpreet Brar</t>
+  </si>
+  <si>
+    <t>Mayank Agarwal</t>
+  </si>
+  <si>
+    <t>Nicholas Pooran</t>
+  </si>
+  <si>
+    <t>Sarfaraz Khan</t>
+  </si>
+  <si>
+    <t>KL Rahul</t>
+  </si>
+  <si>
+    <t>Mandeep Singh</t>
+  </si>
+  <si>
+    <t>Jagadeesha Suchith</t>
+  </si>
+  <si>
+    <t>Mohammad Shami</t>
+  </si>
+  <si>
+    <t>Murugan Ashwin</t>
+  </si>
+  <si>
+    <t>Eoin Morgan</t>
+  </si>
+  <si>
+    <t>Tom Banton</t>
+  </si>
+  <si>
+    <t>Rahul Tripathi</t>
+  </si>
+  <si>
+    <t>Nikhil Shankar Naik</t>
+  </si>
+  <si>
+    <t>Varun Chakaravarthy</t>
+  </si>
+  <si>
+    <t>Chris Green</t>
+  </si>
+  <si>
+    <t>Pravin Tambe</t>
+  </si>
+  <si>
+    <t>M Siddharth</t>
+  </si>
+  <si>
+    <t>Andre Russell</t>
+  </si>
+  <si>
+    <t>Harry Gurney</t>
+  </si>
+  <si>
+    <t>Kamlesh Nagarkoti</t>
+  </si>
+  <si>
+    <t>Lockie Ferguson</t>
+  </si>
+  <si>
+    <t>Nitish Rana</t>
+  </si>
+  <si>
+    <t>Prasidh Krishna</t>
+  </si>
+  <si>
+    <t>Rinku Singh</t>
+  </si>
+  <si>
+    <t>Shubham Gill</t>
+  </si>
+  <si>
+    <t>Siddhesh Lad</t>
+  </si>
+  <si>
+    <t>Dinesh Karthik</t>
+  </si>
+  <si>
+    <t>Sunil Narine</t>
+  </si>
+  <si>
+    <t>Shivam Mavi</t>
+  </si>
+  <si>
+    <t>Kuldeep Yadav</t>
+  </si>
+  <si>
+    <t>Sandeep Warrier</t>
+  </si>
+  <si>
+    <t>Kolkata Knight Riders</t>
+  </si>
+  <si>
+    <t>Robin Uthappa</t>
+  </si>
+  <si>
+    <t>David Miller</t>
+  </si>
+  <si>
+    <t>Anuj Rawat</t>
+  </si>
+  <si>
+    <t>Yashasvi Jaiswal</t>
+  </si>
+  <si>
+    <t>Tom Curran</t>
+  </si>
+  <si>
+    <t>Jaydev Unadkat</t>
+  </si>
+  <si>
+    <t>Kartik Tyagi</t>
+  </si>
+  <si>
+    <t>Andrew Tye</t>
+  </si>
+  <si>
+    <t>Oshane Thomas</t>
+  </si>
+  <si>
+    <t>Anirudha Ashok Joshi</t>
+  </si>
+  <si>
+    <t>Akash Singh</t>
+  </si>
+  <si>
+    <t>Riyan Parag</t>
+  </si>
+  <si>
+    <t>Shashank Singh</t>
+  </si>
+  <si>
+    <t>Steve Smith</t>
+  </si>
+  <si>
+    <t>Manan Vohra</t>
+  </si>
+  <si>
+    <t>Jos Butler</t>
+  </si>
+  <si>
+    <t>Sanju Samson</t>
+  </si>
+  <si>
+    <t>Ben Stokes</t>
+  </si>
+  <si>
+    <t>Mahipal Lomror</t>
+  </si>
+  <si>
+    <t>Shreyas Gopal</t>
+  </si>
+  <si>
+    <t>Ankit Rajpoot</t>
+  </si>
+  <si>
+    <t>Jofra Archer</t>
+  </si>
+  <si>
+    <t>Rahul Tewatia</t>
+  </si>
+  <si>
+    <t>Varun Aaron</t>
+  </si>
+  <si>
+    <t>Rajasthan Royals</t>
+  </si>
+  <si>
+    <t>Priyam Garg</t>
+  </si>
+  <si>
+    <t>Virat Singh</t>
+  </si>
+  <si>
+    <t>Mitchell Marsh</t>
+  </si>
+  <si>
+    <t>Fabian Allen</t>
+  </si>
+  <si>
+    <t>Sandeep Bavanaka</t>
+  </si>
+  <si>
+    <t>Sanjay Yadav</t>
+  </si>
+  <si>
+    <t>Abdul Samad</t>
+  </si>
+  <si>
+    <t>Kane Williamson</t>
+  </si>
+  <si>
+    <t>Abhishek Sharma</t>
+  </si>
+  <si>
+    <t>David Warner</t>
+  </si>
+  <si>
+    <t>Manish Pandey</t>
+  </si>
+  <si>
+    <t>Jonny Bairstow</t>
+  </si>
+  <si>
+    <t>Shreevats Goswami</t>
+  </si>
+  <si>
+    <t>Wridhhiman Saha</t>
+  </si>
+  <si>
+    <t>Vijay Shankar</t>
+  </si>
+  <si>
+    <t>Mohammad Nabi</t>
+  </si>
+  <si>
+    <t>Basil Thampi</t>
+  </si>
+  <si>
+    <t>Bhuvneshwar Kumar</t>
+  </si>
+  <si>
+    <t>Billy Stanlake</t>
+  </si>
+  <si>
+    <t>Rashid Khan</t>
+  </si>
+  <si>
+    <t>Sandeep Sharma</t>
+  </si>
+  <si>
+    <t>Shahbaz Nadeem</t>
+  </si>
+  <si>
+    <t>Siddarth Kaul</t>
+  </si>
+  <si>
+    <t>Syed Khaleel Ahmed</t>
+  </si>
+  <si>
+    <t>T Natarajan</t>
+  </si>
+  <si>
+    <t>Sunrisers Hyderabad</t>
+  </si>
+  <si>
+    <t>AFGANISTAN</t>
+  </si>
+  <si>
+    <t>Delhi Capitals</t>
   </si>
 </sst>
 </file>
@@ -716,7 +1087,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -741,7 +1112,7 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -758,7 +1129,7 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -775,7 +1146,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -792,7 +1163,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -809,7 +1180,7 @@
         <v>9.5</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -826,7 +1197,7 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -843,7 +1214,7 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -860,7 +1231,7 @@
         <v>9.5</v>
       </c>
       <c r="E8" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -877,7 +1248,7 @@
         <v>8.5</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -894,7 +1265,7 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -911,7 +1282,7 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -928,7 +1299,7 @@
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -945,7 +1316,7 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -962,7 +1333,7 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -970,7 +1341,7 @@
         <v>80</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>51</v>
@@ -979,7 +1350,7 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -996,7 +1367,7 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -1013,7 +1384,7 @@
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -1030,7 +1401,7 @@
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -1047,7 +1418,7 @@
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -1064,7 +1435,7 @@
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -1081,7 +1452,7 @@
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -1098,7 +1469,7 @@
         <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -1108,14 +1479,2092 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58CE88C7-9618-F84C-9384-D7C17AFDEA77}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="4" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="5">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="5">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="5">
+        <v>7</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="5">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="5">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="5">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="5">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="5">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="5">
+        <v>8.5</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="5">
+        <v>9</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="5">
+        <v>8</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="5">
+        <v>7</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="5">
+        <v>9</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="5">
+        <v>9</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="5">
+        <v>9</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="5">
+        <v>8</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="5">
+        <v>9</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="5">
+        <v>9</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="5">
+        <v>9</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="5">
+        <v>8</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CB643A-A6C1-D24E-A39C-A304F9BA1AC4}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="45.1640625" customWidth="1"/>
+    <col min="3" max="4" width="37.33203125" customWidth="1"/>
+    <col min="5" max="5" width="51.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="5">
+        <v>9</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="5">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="5">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="5">
+        <v>10</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="5">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="5">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="5">
+        <v>10</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="5">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="5">
+        <v>10</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="5">
+        <v>9</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="5">
+        <v>9</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="5">
+        <v>9</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="5">
+        <v>9</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="5">
+        <v>9</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="5">
+        <v>10</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="5">
+        <v>9</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="5">
+        <v>8</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="5">
+        <v>8</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="5">
+        <v>7</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="5">
+        <v>8</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="5">
+        <v>9</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="5">
+        <v>8</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="5">
+        <v>8</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374C665C-4926-CF4E-93E9-BF149291A71C}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="27" customWidth="1"/>
+    <col min="3" max="4" width="46.5" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="5">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="5">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="5">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="5">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="5">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="5">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="5">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="5">
+        <v>9</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="5">
+        <v>9</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="5">
+        <v>9</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="5">
+        <v>9</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="5">
+        <v>9</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="5">
+        <v>8</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="5">
+        <v>9</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="5">
+        <v>8</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="5">
+        <v>9</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="5">
+        <v>10</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="5">
+        <v>9</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="5">
+        <v>9</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="5">
+        <v>9</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="5">
+        <v>7</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="5">
+        <v>8</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3970B4B3-21D9-C54A-BB87-733CDE66293B}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="31" customWidth="1"/>
+    <col min="3" max="4" width="39" customWidth="1"/>
+    <col min="5" max="5" width="42.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="5">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="5">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="5">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="5">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="5">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="5">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="5">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="5">
+        <v>9</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="5">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="5">
+        <v>9</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="5">
+        <v>9</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="5">
+        <v>9</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="5">
+        <v>8</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="5">
+        <v>10</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="5">
+        <v>9</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="5">
+        <v>8</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="5">
+        <v>9</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="5">
+        <v>8</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="5">
+        <v>8</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="5">
+        <v>7</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB12E93E-59C1-A84E-AA5D-0F545C892CAB}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="35.6640625" customWidth="1"/>
+    <col min="3" max="4" width="34.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="5">
+        <v>9</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="5">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="5">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="5">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="5">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="5">
+        <v>9</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="5">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="5">
+        <v>9</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="5">
+        <v>8</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="5">
+        <v>10</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="5">
+        <v>9</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="5">
+        <v>9</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="5">
+        <v>9</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="5">
+        <v>9</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="5">
+        <v>8</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="5">
+        <v>8</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="5">
+        <v>8</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="5">
+        <v>9</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="5">
+        <v>8</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="5">
+        <v>9</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="5">
+        <v>9</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EAE61C-B86B-1A43-86DD-0D679D0182AB}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>